<commit_message>
sum 22 week 12 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11AF8A9-0E8B-463C-8801-F1400816E528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04926E6F-9AF5-4953-B66B-ACBFEE3D205F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="2625" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="3390" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1129"/>
+  <dimension ref="A1:D1149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1109" workbookViewId="0">
-      <selection activeCell="J1124" sqref="J1124"/>
+    <sheetView tabSelected="1" topLeftCell="A1127" workbookViewId="0">
+      <selection activeCell="A1150" sqref="A1150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16181,6 +16181,286 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1130">
+        <v>5</v>
+      </c>
+      <c r="B1130">
+        <v>1</v>
+      </c>
+      <c r="C1130">
+        <v>4</v>
+      </c>
+      <c r="D1130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1131">
+        <v>3</v>
+      </c>
+      <c r="B1131">
+        <v>1</v>
+      </c>
+      <c r="C1131">
+        <v>3</v>
+      </c>
+      <c r="D1131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1132">
+        <v>5</v>
+      </c>
+      <c r="B1132">
+        <v>0</v>
+      </c>
+      <c r="C1132">
+        <v>5</v>
+      </c>
+      <c r="D1132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1133">
+        <v>6</v>
+      </c>
+      <c r="B1133">
+        <v>3</v>
+      </c>
+      <c r="C1133">
+        <v>3</v>
+      </c>
+      <c r="D1133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1134">
+        <v>3</v>
+      </c>
+      <c r="B1134">
+        <v>2</v>
+      </c>
+      <c r="C1134">
+        <v>2</v>
+      </c>
+      <c r="D1134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1135">
+        <v>3</v>
+      </c>
+      <c r="B1135">
+        <v>2</v>
+      </c>
+      <c r="C1135">
+        <v>2</v>
+      </c>
+      <c r="D1135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1136">
+        <v>6</v>
+      </c>
+      <c r="B1136">
+        <v>0</v>
+      </c>
+      <c r="C1136">
+        <v>6</v>
+      </c>
+      <c r="D1136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1137">
+        <v>3</v>
+      </c>
+      <c r="B1137">
+        <v>3</v>
+      </c>
+      <c r="C1137">
+        <v>3</v>
+      </c>
+      <c r="D1137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1138">
+        <v>6</v>
+      </c>
+      <c r="B1138">
+        <v>2</v>
+      </c>
+      <c r="C1138">
+        <v>6</v>
+      </c>
+      <c r="D1138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1139">
+        <v>3</v>
+      </c>
+      <c r="B1139">
+        <v>1</v>
+      </c>
+      <c r="C1139">
+        <v>3</v>
+      </c>
+      <c r="D1139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1140">
+        <v>4</v>
+      </c>
+      <c r="B1140">
+        <v>2</v>
+      </c>
+      <c r="C1140">
+        <v>3</v>
+      </c>
+      <c r="D1140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1141">
+        <v>3</v>
+      </c>
+      <c r="B1141">
+        <v>3</v>
+      </c>
+      <c r="C1141">
+        <v>3</v>
+      </c>
+      <c r="D1141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1142">
+        <v>4</v>
+      </c>
+      <c r="B1142">
+        <v>3</v>
+      </c>
+      <c r="C1142">
+        <v>4</v>
+      </c>
+      <c r="D1142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1143">
+        <v>6</v>
+      </c>
+      <c r="B1143">
+        <v>2</v>
+      </c>
+      <c r="C1143">
+        <v>5</v>
+      </c>
+      <c r="D1143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1144">
+        <v>5</v>
+      </c>
+      <c r="B1144">
+        <v>2</v>
+      </c>
+      <c r="C1144">
+        <v>6</v>
+      </c>
+      <c r="D1144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1145">
+        <v>5</v>
+      </c>
+      <c r="B1145">
+        <v>2</v>
+      </c>
+      <c r="C1145">
+        <v>5</v>
+      </c>
+      <c r="D1145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1146">
+        <v>4</v>
+      </c>
+      <c r="B1146">
+        <v>0</v>
+      </c>
+      <c r="C1146">
+        <v>4</v>
+      </c>
+      <c r="D1146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1147">
+        <v>2</v>
+      </c>
+      <c r="B1147">
+        <v>3</v>
+      </c>
+      <c r="C1147">
+        <v>3</v>
+      </c>
+      <c r="D1147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1148">
+        <v>6</v>
+      </c>
+      <c r="B1148">
+        <v>3</v>
+      </c>
+      <c r="C1148">
+        <v>5</v>
+      </c>
+      <c r="D1148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1149">
+        <v>4</v>
+      </c>
+      <c r="B1149">
+        <v>0</v>
+      </c>
+      <c r="C1149">
+        <v>5</v>
+      </c>
+      <c r="D1149">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
summer 2022 week 15 games
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88237A53-07F4-41A6-9BDD-4DC3C6005DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A837E431-42D9-414D-B974-27904913079C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="-3195" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2625" yWindow="1155" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1130"/>
+  <dimension ref="A1:D1150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1112" workbookViewId="0">
-      <selection activeCell="A1131" sqref="A1131"/>
+    <sheetView tabSelected="1" topLeftCell="A1127" workbookViewId="0">
+      <selection activeCell="H1136" sqref="H1136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16195,6 +16195,286 @@
         <v>2</v>
       </c>
     </row>
+    <row r="1131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1131">
+        <v>5</v>
+      </c>
+      <c r="B1131">
+        <v>2</v>
+      </c>
+      <c r="C1131">
+        <v>3</v>
+      </c>
+      <c r="D1131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1132">
+        <v>3</v>
+      </c>
+      <c r="B1132">
+        <v>1</v>
+      </c>
+      <c r="C1132">
+        <v>3</v>
+      </c>
+      <c r="D1132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1133">
+        <v>5</v>
+      </c>
+      <c r="B1133">
+        <v>0</v>
+      </c>
+      <c r="C1133">
+        <v>5</v>
+      </c>
+      <c r="D1133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1134">
+        <v>4</v>
+      </c>
+      <c r="B1134">
+        <v>1</v>
+      </c>
+      <c r="C1134">
+        <v>4</v>
+      </c>
+      <c r="D1134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1135">
+        <v>6</v>
+      </c>
+      <c r="B1135">
+        <v>1</v>
+      </c>
+      <c r="C1135">
+        <v>6</v>
+      </c>
+      <c r="D1135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1136">
+        <v>4</v>
+      </c>
+      <c r="B1136">
+        <v>2</v>
+      </c>
+      <c r="C1136">
+        <v>4</v>
+      </c>
+      <c r="D1136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1137">
+        <v>3</v>
+      </c>
+      <c r="B1137">
+        <v>0</v>
+      </c>
+      <c r="C1137">
+        <v>3</v>
+      </c>
+      <c r="D1137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1138">
+        <v>5</v>
+      </c>
+      <c r="B1138">
+        <v>2</v>
+      </c>
+      <c r="C1138">
+        <v>4</v>
+      </c>
+      <c r="D1138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1139">
+        <v>6</v>
+      </c>
+      <c r="B1139">
+        <v>2</v>
+      </c>
+      <c r="C1139">
+        <v>6</v>
+      </c>
+      <c r="D1139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1140">
+        <v>3</v>
+      </c>
+      <c r="B1140">
+        <v>1</v>
+      </c>
+      <c r="C1140">
+        <v>6</v>
+      </c>
+      <c r="D1140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1141">
+        <v>7</v>
+      </c>
+      <c r="B1141">
+        <v>2</v>
+      </c>
+      <c r="C1141">
+        <v>5</v>
+      </c>
+      <c r="D1141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1142">
+        <v>3</v>
+      </c>
+      <c r="B1142">
+        <v>1</v>
+      </c>
+      <c r="C1142">
+        <v>4</v>
+      </c>
+      <c r="D1142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1143">
+        <v>2</v>
+      </c>
+      <c r="B1143">
+        <v>0</v>
+      </c>
+      <c r="C1143">
+        <v>2</v>
+      </c>
+      <c r="D1143">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1144">
+        <v>3</v>
+      </c>
+      <c r="B1144">
+        <v>2</v>
+      </c>
+      <c r="C1144">
+        <v>5</v>
+      </c>
+      <c r="D1144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1145">
+        <v>7</v>
+      </c>
+      <c r="B1145">
+        <v>3</v>
+      </c>
+      <c r="C1145">
+        <v>5</v>
+      </c>
+      <c r="D1145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1146">
+        <v>6</v>
+      </c>
+      <c r="B1146">
+        <v>0</v>
+      </c>
+      <c r="C1146">
+        <v>5</v>
+      </c>
+      <c r="D1146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1147">
+        <v>3</v>
+      </c>
+      <c r="B1147">
+        <v>0</v>
+      </c>
+      <c r="C1147">
+        <v>3</v>
+      </c>
+      <c r="D1147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1148">
+        <v>2</v>
+      </c>
+      <c r="B1148">
+        <v>2</v>
+      </c>
+      <c r="C1148">
+        <v>2</v>
+      </c>
+      <c r="D1148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1149">
+        <v>6</v>
+      </c>
+      <c r="B1149">
+        <v>3</v>
+      </c>
+      <c r="C1149">
+        <v>7</v>
+      </c>
+      <c r="D1149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1150">
+        <v>4</v>
+      </c>
+      <c r="B1150">
+        <v>0</v>
+      </c>
+      <c r="C1150">
+        <v>2</v>
+      </c>
+      <c r="D1150">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
week 3 inn inputs week 3 results inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C03317-B393-434B-BB84-BDB6EB7B367A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80DCC74-A83A-4620-ABB9-8EE8E2BF2212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20865" yWindow="1425" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1216"/>
+  <dimension ref="A1:D1241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1193" workbookViewId="0">
-      <selection activeCell="E1204" sqref="E1204"/>
+    <sheetView tabSelected="1" topLeftCell="A1214" workbookViewId="0">
+      <selection activeCell="A1242" sqref="A1242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17399,6 +17399,356 @@
         <v>3</v>
       </c>
     </row>
+    <row r="1217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1217">
+        <v>7</v>
+      </c>
+      <c r="B1217">
+        <v>3</v>
+      </c>
+      <c r="C1217">
+        <v>6</v>
+      </c>
+      <c r="D1217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1218">
+        <v>4</v>
+      </c>
+      <c r="B1218">
+        <v>3</v>
+      </c>
+      <c r="C1218">
+        <v>2</v>
+      </c>
+      <c r="D1218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1219">
+        <v>3</v>
+      </c>
+      <c r="B1219">
+        <v>3</v>
+      </c>
+      <c r="C1219">
+        <v>6</v>
+      </c>
+      <c r="D1219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1220">
+        <v>2</v>
+      </c>
+      <c r="B1220">
+        <v>1</v>
+      </c>
+      <c r="C1220">
+        <v>3</v>
+      </c>
+      <c r="D1220">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1221">
+        <v>7</v>
+      </c>
+      <c r="B1221">
+        <v>2</v>
+      </c>
+      <c r="C1221">
+        <v>2</v>
+      </c>
+      <c r="D1221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1222">
+        <v>3</v>
+      </c>
+      <c r="B1222">
+        <v>0</v>
+      </c>
+      <c r="C1222">
+        <v>3</v>
+      </c>
+      <c r="D1222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1223">
+        <v>6</v>
+      </c>
+      <c r="B1223">
+        <v>0</v>
+      </c>
+      <c r="C1223">
+        <v>6</v>
+      </c>
+      <c r="D1223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1224">
+        <v>3</v>
+      </c>
+      <c r="B1224">
+        <v>1</v>
+      </c>
+      <c r="C1224">
+        <v>4</v>
+      </c>
+      <c r="D1224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1225">
+        <v>2</v>
+      </c>
+      <c r="B1225">
+        <v>2</v>
+      </c>
+      <c r="C1225">
+        <v>2</v>
+      </c>
+      <c r="D1225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1226">
+        <v>3</v>
+      </c>
+      <c r="B1226">
+        <v>3</v>
+      </c>
+      <c r="C1226">
+        <v>6</v>
+      </c>
+      <c r="D1226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1227">
+        <v>6</v>
+      </c>
+      <c r="B1227">
+        <v>2</v>
+      </c>
+      <c r="C1227">
+        <v>5</v>
+      </c>
+      <c r="D1227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1228">
+        <v>4</v>
+      </c>
+      <c r="B1228">
+        <v>0</v>
+      </c>
+      <c r="C1228">
+        <v>5</v>
+      </c>
+      <c r="D1228">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1229">
+        <v>3</v>
+      </c>
+      <c r="B1229">
+        <v>3</v>
+      </c>
+      <c r="C1229">
+        <v>3</v>
+      </c>
+      <c r="D1229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1230">
+        <v>3</v>
+      </c>
+      <c r="B1230">
+        <v>2</v>
+      </c>
+      <c r="C1230">
+        <v>4</v>
+      </c>
+      <c r="D1230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1231">
+        <v>6</v>
+      </c>
+      <c r="B1231">
+        <v>0</v>
+      </c>
+      <c r="C1231">
+        <v>6</v>
+      </c>
+      <c r="D1231">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1232">
+        <v>5</v>
+      </c>
+      <c r="B1232">
+        <v>0</v>
+      </c>
+      <c r="C1232">
+        <v>4</v>
+      </c>
+      <c r="D1232">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1233">
+        <v>5</v>
+      </c>
+      <c r="B1233">
+        <v>2</v>
+      </c>
+      <c r="C1233">
+        <v>6</v>
+      </c>
+      <c r="D1233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1234">
+        <v>2</v>
+      </c>
+      <c r="B1234">
+        <v>1</v>
+      </c>
+      <c r="C1234">
+        <v>3</v>
+      </c>
+      <c r="D1234">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1235">
+        <v>5</v>
+      </c>
+      <c r="B1235">
+        <v>0</v>
+      </c>
+      <c r="C1235">
+        <v>5</v>
+      </c>
+      <c r="D1235">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1236">
+        <v>6</v>
+      </c>
+      <c r="B1236">
+        <v>2</v>
+      </c>
+      <c r="C1236">
+        <v>4</v>
+      </c>
+      <c r="D1236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1237">
+        <v>2</v>
+      </c>
+      <c r="B1237">
+        <v>0</v>
+      </c>
+      <c r="C1237">
+        <v>3</v>
+      </c>
+      <c r="D1237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1238">
+        <v>6</v>
+      </c>
+      <c r="B1238">
+        <v>1</v>
+      </c>
+      <c r="C1238">
+        <v>5</v>
+      </c>
+      <c r="D1238">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1239">
+        <v>4</v>
+      </c>
+      <c r="B1239">
+        <v>0</v>
+      </c>
+      <c r="C1239">
+        <v>3</v>
+      </c>
+      <c r="D1239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1240">
+        <v>6</v>
+      </c>
+      <c r="B1240">
+        <v>2</v>
+      </c>
+      <c r="C1240">
+        <v>7</v>
+      </c>
+      <c r="D1240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1241">
+        <v>4</v>
+      </c>
+      <c r="B1241">
+        <v>2</v>
+      </c>
+      <c r="C1241">
+        <v>5</v>
+      </c>
+      <c r="D1241">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fall 22 week 8 complete and team calendar command
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B109B7-7DFC-4972-9CA4-A96B1AE4AD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030204AF-EB93-45C0-8A2A-E85A0BA5A4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="0" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19335" yWindow="2400" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1337"/>
+  <dimension ref="A1:D1361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1313" workbookViewId="0">
-      <selection activeCell="A1338" sqref="A1338"/>
+    <sheetView tabSelected="1" topLeftCell="A1349" workbookViewId="0">
+      <selection activeCell="A1362" sqref="A1362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19093,6 +19093,342 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1338">
+        <v>4</v>
+      </c>
+      <c r="B1338">
+        <v>0</v>
+      </c>
+      <c r="C1338">
+        <v>4</v>
+      </c>
+      <c r="D1338">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1339">
+        <v>5</v>
+      </c>
+      <c r="B1339">
+        <v>2</v>
+      </c>
+      <c r="C1339">
+        <v>5</v>
+      </c>
+      <c r="D1339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1340">
+        <v>3</v>
+      </c>
+      <c r="B1340">
+        <v>2</v>
+      </c>
+      <c r="C1340">
+        <v>4</v>
+      </c>
+      <c r="D1340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1341">
+        <v>3</v>
+      </c>
+      <c r="B1341">
+        <v>2</v>
+      </c>
+      <c r="C1341">
+        <v>3</v>
+      </c>
+      <c r="D1341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1342">
+        <v>7</v>
+      </c>
+      <c r="B1342">
+        <v>2</v>
+      </c>
+      <c r="C1342">
+        <v>5</v>
+      </c>
+      <c r="D1342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1343">
+        <v>5</v>
+      </c>
+      <c r="B1343">
+        <v>2</v>
+      </c>
+      <c r="C1343">
+        <v>4</v>
+      </c>
+      <c r="D1343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1344">
+        <v>4</v>
+      </c>
+      <c r="B1344">
+        <v>3</v>
+      </c>
+      <c r="C1344">
+        <v>3</v>
+      </c>
+      <c r="D1344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1345">
+        <v>4</v>
+      </c>
+      <c r="B1345">
+        <v>1</v>
+      </c>
+      <c r="C1345">
+        <v>6</v>
+      </c>
+      <c r="D1345">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1346">
+        <v>6</v>
+      </c>
+      <c r="B1346">
+        <v>2</v>
+      </c>
+      <c r="C1346">
+        <v>7</v>
+      </c>
+      <c r="D1346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1347">
+        <v>2</v>
+      </c>
+      <c r="B1347">
+        <v>1</v>
+      </c>
+      <c r="C1347">
+        <v>3</v>
+      </c>
+      <c r="D1347">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1348">
+        <v>3</v>
+      </c>
+      <c r="B1348">
+        <v>1</v>
+      </c>
+      <c r="C1348">
+        <v>4</v>
+      </c>
+      <c r="D1348">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1349">
+        <v>6</v>
+      </c>
+      <c r="B1349">
+        <v>0</v>
+      </c>
+      <c r="C1349">
+        <v>6</v>
+      </c>
+      <c r="D1349">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1350">
+        <v>5</v>
+      </c>
+      <c r="B1350">
+        <v>2</v>
+      </c>
+      <c r="C1350">
+        <v>5</v>
+      </c>
+      <c r="D1350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1351">
+        <v>5</v>
+      </c>
+      <c r="B1351">
+        <v>0</v>
+      </c>
+      <c r="C1351">
+        <v>4</v>
+      </c>
+      <c r="D1351">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1352">
+        <v>4</v>
+      </c>
+      <c r="B1352">
+        <v>2</v>
+      </c>
+      <c r="C1352">
+        <v>4</v>
+      </c>
+      <c r="D1352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1353">
+        <v>5</v>
+      </c>
+      <c r="B1353">
+        <v>3</v>
+      </c>
+      <c r="C1353">
+        <v>4</v>
+      </c>
+      <c r="D1353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1354">
+        <v>5</v>
+      </c>
+      <c r="B1354">
+        <v>2</v>
+      </c>
+      <c r="C1354">
+        <v>5</v>
+      </c>
+      <c r="D1354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1355">
+        <v>6</v>
+      </c>
+      <c r="B1355">
+        <v>1</v>
+      </c>
+      <c r="C1355">
+        <v>6</v>
+      </c>
+      <c r="D1355">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1356">
+        <v>3</v>
+      </c>
+      <c r="B1356">
+        <v>2</v>
+      </c>
+      <c r="C1356">
+        <v>4</v>
+      </c>
+      <c r="D1356">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1357">
+        <v>4</v>
+      </c>
+      <c r="B1357">
+        <v>1</v>
+      </c>
+      <c r="C1357">
+        <v>4</v>
+      </c>
+      <c r="D1357">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1358">
+        <v>6</v>
+      </c>
+      <c r="B1358">
+        <v>0</v>
+      </c>
+      <c r="C1358">
+        <v>5</v>
+      </c>
+      <c r="D1358">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1359">
+        <v>6</v>
+      </c>
+      <c r="B1359">
+        <v>3</v>
+      </c>
+      <c r="C1359">
+        <v>5</v>
+      </c>
+      <c r="D1359">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1360">
+        <v>3</v>
+      </c>
+      <c r="B1360">
+        <v>2</v>
+      </c>
+      <c r="C1360">
+        <v>5</v>
+      </c>
+      <c r="D1360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1361">
+        <v>5</v>
+      </c>
+      <c r="B1361">
+        <v>0</v>
+      </c>
+      <c r="C1361">
+        <v>5</v>
+      </c>
+      <c r="D1361">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fall 22 week 9 complete
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030204AF-EB93-45C0-8A2A-E85A0BA5A4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AB829A-F007-4CB2-8CF7-32293D91C017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19335" yWindow="2400" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="2160" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1361"/>
+  <dimension ref="A1:D1384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1349" workbookViewId="0">
-      <selection activeCell="A1362" sqref="A1362"/>
+    <sheetView tabSelected="1" topLeftCell="A1361" workbookViewId="0">
+      <selection activeCell="A1385" sqref="A1385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19429,6 +19429,328 @@
         <v>2</v>
       </c>
     </row>
+    <row r="1362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1362">
+        <v>3</v>
+      </c>
+      <c r="B1362">
+        <v>0</v>
+      </c>
+      <c r="C1362">
+        <v>7</v>
+      </c>
+      <c r="D1362">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1363">
+        <v>4</v>
+      </c>
+      <c r="B1363">
+        <v>2</v>
+      </c>
+      <c r="C1363">
+        <v>3</v>
+      </c>
+      <c r="D1363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1364">
+        <v>4</v>
+      </c>
+      <c r="B1364">
+        <v>2</v>
+      </c>
+      <c r="C1364">
+        <v>5</v>
+      </c>
+      <c r="D1364">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1365">
+        <v>3</v>
+      </c>
+      <c r="B1365">
+        <v>2</v>
+      </c>
+      <c r="C1365">
+        <v>3</v>
+      </c>
+      <c r="D1365">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1366">
+        <v>6</v>
+      </c>
+      <c r="B1366">
+        <v>3</v>
+      </c>
+      <c r="C1366">
+        <v>2</v>
+      </c>
+      <c r="D1366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1367">
+        <v>3</v>
+      </c>
+      <c r="B1367">
+        <v>0</v>
+      </c>
+      <c r="C1367">
+        <v>2</v>
+      </c>
+      <c r="D1367">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1368">
+        <v>6</v>
+      </c>
+      <c r="B1368">
+        <v>2</v>
+      </c>
+      <c r="C1368">
+        <v>5</v>
+      </c>
+      <c r="D1368">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1369">
+        <v>4</v>
+      </c>
+      <c r="B1369">
+        <v>0</v>
+      </c>
+      <c r="C1369">
+        <v>3</v>
+      </c>
+      <c r="D1369">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1370">
+        <v>7</v>
+      </c>
+      <c r="B1370">
+        <v>1</v>
+      </c>
+      <c r="C1370">
+        <v>6</v>
+      </c>
+      <c r="D1370">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1371">
+        <v>3</v>
+      </c>
+      <c r="B1371">
+        <v>1</v>
+      </c>
+      <c r="C1371">
+        <v>4</v>
+      </c>
+      <c r="D1371">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1372">
+        <v>5</v>
+      </c>
+      <c r="B1372">
+        <v>2</v>
+      </c>
+      <c r="C1372">
+        <v>5</v>
+      </c>
+      <c r="D1372">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1373">
+        <v>3</v>
+      </c>
+      <c r="B1373">
+        <v>2</v>
+      </c>
+      <c r="C1373">
+        <v>4</v>
+      </c>
+      <c r="D1373">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1374">
+        <v>4</v>
+      </c>
+      <c r="B1374">
+        <v>0</v>
+      </c>
+      <c r="C1374">
+        <v>6</v>
+      </c>
+      <c r="D1374">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1375">
+        <v>4</v>
+      </c>
+      <c r="B1375">
+        <v>2</v>
+      </c>
+      <c r="C1375">
+        <v>2</v>
+      </c>
+      <c r="D1375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1376">
+        <v>5</v>
+      </c>
+      <c r="B1376">
+        <v>0</v>
+      </c>
+      <c r="C1376">
+        <v>6</v>
+      </c>
+      <c r="D1376">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1377">
+        <v>4</v>
+      </c>
+      <c r="B1377">
+        <v>0</v>
+      </c>
+      <c r="C1377">
+        <v>3</v>
+      </c>
+      <c r="D1377">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1378">
+        <v>6</v>
+      </c>
+      <c r="B1378">
+        <v>0</v>
+      </c>
+      <c r="C1378">
+        <v>6</v>
+      </c>
+      <c r="D1378">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1379">
+        <v>4</v>
+      </c>
+      <c r="B1379">
+        <v>0</v>
+      </c>
+      <c r="C1379">
+        <v>3</v>
+      </c>
+      <c r="D1379">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1380">
+        <v>4</v>
+      </c>
+      <c r="B1380">
+        <v>2</v>
+      </c>
+      <c r="C1380">
+        <v>2</v>
+      </c>
+      <c r="D1380">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1381">
+        <v>5</v>
+      </c>
+      <c r="B1381">
+        <v>3</v>
+      </c>
+      <c r="C1381">
+        <v>3</v>
+      </c>
+      <c r="D1381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1382">
+        <v>5</v>
+      </c>
+      <c r="B1382">
+        <v>2</v>
+      </c>
+      <c r="C1382">
+        <v>3</v>
+      </c>
+      <c r="D1382">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1383">
+        <v>4</v>
+      </c>
+      <c r="B1383">
+        <v>0</v>
+      </c>
+      <c r="C1383">
+        <v>5</v>
+      </c>
+      <c r="D1383">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1384">
+        <v>6</v>
+      </c>
+      <c r="B1384">
+        <v>0</v>
+      </c>
+      <c r="C1384">
+        <v>7</v>
+      </c>
+      <c r="D1384">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fall 22 week 10 complete
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AB829A-F007-4CB2-8CF7-32293D91C017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDB09C1-6762-40CB-A488-72401189D0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2160" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1384"/>
+  <dimension ref="A1:D1408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1361" workbookViewId="0">
-      <selection activeCell="A1385" sqref="A1385"/>
+    <sheetView tabSelected="1" topLeftCell="A1385" workbookViewId="0">
+      <selection activeCell="A1409" sqref="A1409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19751,6 +19751,342 @@
         <v>2</v>
       </c>
     </row>
+    <row r="1385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1385">
+        <v>4</v>
+      </c>
+      <c r="B1385">
+        <v>2</v>
+      </c>
+      <c r="C1385">
+        <v>4</v>
+      </c>
+      <c r="D1385">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1386">
+        <v>3</v>
+      </c>
+      <c r="B1386">
+        <v>2</v>
+      </c>
+      <c r="C1386">
+        <v>2</v>
+      </c>
+      <c r="D1386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1387">
+        <v>5</v>
+      </c>
+      <c r="B1387">
+        <v>0</v>
+      </c>
+      <c r="C1387">
+        <v>4</v>
+      </c>
+      <c r="D1387">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1388">
+        <v>3</v>
+      </c>
+      <c r="B1388">
+        <v>0</v>
+      </c>
+      <c r="C1388">
+        <v>3</v>
+      </c>
+      <c r="D1388">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1389">
+        <v>4</v>
+      </c>
+      <c r="B1389">
+        <v>0</v>
+      </c>
+      <c r="C1389">
+        <v>5</v>
+      </c>
+      <c r="D1389">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1390">
+        <v>4</v>
+      </c>
+      <c r="B1390">
+        <v>3</v>
+      </c>
+      <c r="C1390">
+        <v>4</v>
+      </c>
+      <c r="D1390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1391">
+        <v>5</v>
+      </c>
+      <c r="B1391">
+        <v>0</v>
+      </c>
+      <c r="C1391">
+        <v>6</v>
+      </c>
+      <c r="D1391">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1392">
+        <v>4</v>
+      </c>
+      <c r="B1392">
+        <v>0</v>
+      </c>
+      <c r="C1392">
+        <v>7</v>
+      </c>
+      <c r="D1392">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1393">
+        <v>5</v>
+      </c>
+      <c r="B1393">
+        <v>3</v>
+      </c>
+      <c r="C1393">
+        <v>3</v>
+      </c>
+      <c r="D1393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1394">
+        <v>5</v>
+      </c>
+      <c r="B1394">
+        <v>3</v>
+      </c>
+      <c r="C1394">
+        <v>3</v>
+      </c>
+      <c r="D1394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1395">
+        <v>6</v>
+      </c>
+      <c r="B1395">
+        <v>0</v>
+      </c>
+      <c r="C1395">
+        <v>5</v>
+      </c>
+      <c r="D1395">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1396">
+        <v>5</v>
+      </c>
+      <c r="B1396">
+        <v>0</v>
+      </c>
+      <c r="C1396">
+        <v>4</v>
+      </c>
+      <c r="D1396">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1397">
+        <v>5</v>
+      </c>
+      <c r="B1397">
+        <v>2</v>
+      </c>
+      <c r="C1397">
+        <v>6</v>
+      </c>
+      <c r="D1397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1398">
+        <v>4</v>
+      </c>
+      <c r="B1398">
+        <v>2</v>
+      </c>
+      <c r="C1398">
+        <v>4</v>
+      </c>
+      <c r="D1398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1399">
+        <v>2</v>
+      </c>
+      <c r="B1399">
+        <v>3</v>
+      </c>
+      <c r="C1399">
+        <v>3</v>
+      </c>
+      <c r="D1399">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1400">
+        <v>4</v>
+      </c>
+      <c r="B1400">
+        <v>1</v>
+      </c>
+      <c r="C1400">
+        <v>5</v>
+      </c>
+      <c r="D1400">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1401">
+        <v>4</v>
+      </c>
+      <c r="B1401">
+        <v>2</v>
+      </c>
+      <c r="C1401">
+        <v>4</v>
+      </c>
+      <c r="D1401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1402">
+        <v>6</v>
+      </c>
+      <c r="B1402">
+        <v>2</v>
+      </c>
+      <c r="C1402">
+        <v>6</v>
+      </c>
+      <c r="D1402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1403">
+        <v>5</v>
+      </c>
+      <c r="B1403">
+        <v>2</v>
+      </c>
+      <c r="C1403">
+        <v>5</v>
+      </c>
+      <c r="D1403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1404">
+        <v>3</v>
+      </c>
+      <c r="B1404">
+        <v>3</v>
+      </c>
+      <c r="C1404">
+        <v>3</v>
+      </c>
+      <c r="D1404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1405">
+        <v>3</v>
+      </c>
+      <c r="B1405">
+        <v>0</v>
+      </c>
+      <c r="C1405">
+        <v>5</v>
+      </c>
+      <c r="D1405">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1406">
+        <v>3</v>
+      </c>
+      <c r="B1406">
+        <v>3</v>
+      </c>
+      <c r="C1406">
+        <v>2</v>
+      </c>
+      <c r="D1406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1407">
+        <v>3</v>
+      </c>
+      <c r="B1407">
+        <v>1</v>
+      </c>
+      <c r="C1407">
+        <v>4</v>
+      </c>
+      <c r="D1407">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1408">
+        <v>5</v>
+      </c>
+      <c r="B1408">
+        <v>1</v>
+      </c>
+      <c r="C1408">
+        <v>5</v>
+      </c>
+      <c r="D1408">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fall 22 week 15 complete
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FA1323-A473-45C3-A58D-4EF1E7232DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C7AC01-1E91-4A2D-A032-7B53C4CE4F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1502"/>
+  <dimension ref="A1:D1524"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1476" workbookViewId="0">
-      <selection activeCell="A1503" sqref="A1503"/>
+    <sheetView tabSelected="1" topLeftCell="A1512" workbookViewId="0">
+      <selection activeCell="A1525" sqref="A1525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21403,6 +21403,314 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1503">
+        <v>4</v>
+      </c>
+      <c r="B1503">
+        <v>1</v>
+      </c>
+      <c r="C1503">
+        <v>4</v>
+      </c>
+      <c r="D1503">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1504">
+        <v>2</v>
+      </c>
+      <c r="B1504">
+        <v>1</v>
+      </c>
+      <c r="C1504">
+        <v>2</v>
+      </c>
+      <c r="D1504">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1505">
+        <v>7</v>
+      </c>
+      <c r="B1505">
+        <v>0</v>
+      </c>
+      <c r="C1505">
+        <v>5</v>
+      </c>
+      <c r="D1505">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1506">
+        <v>7</v>
+      </c>
+      <c r="B1506">
+        <v>2</v>
+      </c>
+      <c r="C1506">
+        <v>6</v>
+      </c>
+      <c r="D1506">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1507">
+        <v>3</v>
+      </c>
+      <c r="B1507">
+        <v>0</v>
+      </c>
+      <c r="C1507">
+        <v>5</v>
+      </c>
+      <c r="D1507">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1508">
+        <v>5</v>
+      </c>
+      <c r="B1508">
+        <v>2</v>
+      </c>
+      <c r="C1508">
+        <v>5</v>
+      </c>
+      <c r="D1508">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1509">
+        <v>6</v>
+      </c>
+      <c r="B1509">
+        <v>2</v>
+      </c>
+      <c r="C1509">
+        <v>5</v>
+      </c>
+      <c r="D1509">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1510">
+        <v>2</v>
+      </c>
+      <c r="B1510">
+        <v>2</v>
+      </c>
+      <c r="C1510">
+        <v>5</v>
+      </c>
+      <c r="D1510">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1511">
+        <v>6</v>
+      </c>
+      <c r="B1511">
+        <v>2</v>
+      </c>
+      <c r="C1511">
+        <v>4</v>
+      </c>
+      <c r="D1511">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1512">
+        <v>4</v>
+      </c>
+      <c r="B1512">
+        <v>0</v>
+      </c>
+      <c r="C1512">
+        <v>4</v>
+      </c>
+      <c r="D1512">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1513">
+        <v>4</v>
+      </c>
+      <c r="B1513">
+        <v>3</v>
+      </c>
+      <c r="C1513">
+        <v>4</v>
+      </c>
+      <c r="D1513">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1514">
+        <v>4</v>
+      </c>
+      <c r="B1514">
+        <v>1</v>
+      </c>
+      <c r="C1514">
+        <v>4</v>
+      </c>
+      <c r="D1514">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1515">
+        <v>5</v>
+      </c>
+      <c r="B1515">
+        <v>0</v>
+      </c>
+      <c r="C1515">
+        <v>5</v>
+      </c>
+      <c r="D1515">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1516">
+        <v>3</v>
+      </c>
+      <c r="B1516">
+        <v>1</v>
+      </c>
+      <c r="C1516">
+        <v>2</v>
+      </c>
+      <c r="D1516">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1517">
+        <v>4</v>
+      </c>
+      <c r="B1517">
+        <v>0</v>
+      </c>
+      <c r="C1517">
+        <v>3</v>
+      </c>
+      <c r="D1517">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1518">
+        <v>5</v>
+      </c>
+      <c r="B1518">
+        <v>0</v>
+      </c>
+      <c r="C1518">
+        <v>4</v>
+      </c>
+      <c r="D1518">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1519">
+        <v>4</v>
+      </c>
+      <c r="B1519">
+        <v>0</v>
+      </c>
+      <c r="C1519">
+        <v>7</v>
+      </c>
+      <c r="D1519">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1520">
+        <v>6</v>
+      </c>
+      <c r="B1520">
+        <v>0</v>
+      </c>
+      <c r="C1520">
+        <v>5</v>
+      </c>
+      <c r="D1520">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1521">
+        <v>6</v>
+      </c>
+      <c r="B1521">
+        <v>2</v>
+      </c>
+      <c r="C1521">
+        <v>6</v>
+      </c>
+      <c r="D1521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1522">
+        <v>3</v>
+      </c>
+      <c r="B1522">
+        <v>2</v>
+      </c>
+      <c r="C1522">
+        <v>6</v>
+      </c>
+      <c r="D1522">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1523">
+        <v>5</v>
+      </c>
+      <c r="B1523">
+        <v>2</v>
+      </c>
+      <c r="C1523">
+        <v>4</v>
+      </c>
+      <c r="D1523">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1524">
+        <v>5</v>
+      </c>
+      <c r="B1524">
+        <v>0</v>
+      </c>
+      <c r="C1524">
+        <v>2</v>
+      </c>
+      <c r="D1524">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fall 22 regular session complete
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C7AC01-1E91-4A2D-A032-7B53C4CE4F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2B5410-2812-4E89-8583-52398FBB4B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1524"/>
+  <dimension ref="A1:D1547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1512" workbookViewId="0">
-      <selection activeCell="A1525" sqref="A1525"/>
+    <sheetView tabSelected="1" topLeftCell="A1545" workbookViewId="0">
+      <selection activeCell="A1548" sqref="A1548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21711,6 +21711,328 @@
         <v>2</v>
       </c>
     </row>
+    <row r="1525" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1525">
+        <v>5</v>
+      </c>
+      <c r="B1525">
+        <v>1</v>
+      </c>
+      <c r="C1525">
+        <v>4</v>
+      </c>
+      <c r="D1525">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1526">
+        <v>5</v>
+      </c>
+      <c r="B1526">
+        <v>0</v>
+      </c>
+      <c r="C1526">
+        <v>7</v>
+      </c>
+      <c r="D1526">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1527">
+        <v>5</v>
+      </c>
+      <c r="B1527">
+        <v>0</v>
+      </c>
+      <c r="C1527">
+        <v>5</v>
+      </c>
+      <c r="D1527">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1528">
+        <v>6</v>
+      </c>
+      <c r="B1528">
+        <v>0</v>
+      </c>
+      <c r="C1528">
+        <v>6</v>
+      </c>
+      <c r="D1528">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1529">
+        <v>4</v>
+      </c>
+      <c r="B1529">
+        <v>0</v>
+      </c>
+      <c r="C1529">
+        <v>4</v>
+      </c>
+      <c r="D1529">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1530">
+        <v>4</v>
+      </c>
+      <c r="B1530">
+        <v>1</v>
+      </c>
+      <c r="C1530">
+        <v>4</v>
+      </c>
+      <c r="D1530">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1531">
+        <v>4</v>
+      </c>
+      <c r="B1531">
+        <v>1</v>
+      </c>
+      <c r="C1531">
+        <v>4</v>
+      </c>
+      <c r="D1531">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1532">
+        <v>5</v>
+      </c>
+      <c r="B1532">
+        <v>2</v>
+      </c>
+      <c r="C1532">
+        <v>3</v>
+      </c>
+      <c r="D1532">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1533">
+        <v>3</v>
+      </c>
+      <c r="B1533">
+        <v>2</v>
+      </c>
+      <c r="C1533">
+        <v>4</v>
+      </c>
+      <c r="D1533">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1534">
+        <v>6</v>
+      </c>
+      <c r="B1534">
+        <v>0</v>
+      </c>
+      <c r="C1534">
+        <v>4</v>
+      </c>
+      <c r="D1534">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1535">
+        <v>3</v>
+      </c>
+      <c r="B1535">
+        <v>3</v>
+      </c>
+      <c r="C1535">
+        <v>3</v>
+      </c>
+      <c r="D1535">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1536">
+        <v>3</v>
+      </c>
+      <c r="B1536">
+        <v>2</v>
+      </c>
+      <c r="C1536">
+        <v>4</v>
+      </c>
+      <c r="D1536">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1537">
+        <v>7</v>
+      </c>
+      <c r="B1537">
+        <v>0</v>
+      </c>
+      <c r="C1537">
+        <v>5</v>
+      </c>
+      <c r="D1537">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1538">
+        <v>4</v>
+      </c>
+      <c r="B1538">
+        <v>1</v>
+      </c>
+      <c r="C1538">
+        <v>4</v>
+      </c>
+      <c r="D1538">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1539">
+        <v>3</v>
+      </c>
+      <c r="B1539">
+        <v>2</v>
+      </c>
+      <c r="C1539">
+        <v>3</v>
+      </c>
+      <c r="D1539">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1540">
+        <v>6</v>
+      </c>
+      <c r="B1540">
+        <v>2</v>
+      </c>
+      <c r="C1540">
+        <v>6</v>
+      </c>
+      <c r="D1540">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1541">
+        <v>6</v>
+      </c>
+      <c r="B1541">
+        <v>2</v>
+      </c>
+      <c r="C1541">
+        <v>6</v>
+      </c>
+      <c r="D1541">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1542">
+        <v>2</v>
+      </c>
+      <c r="B1542">
+        <v>2</v>
+      </c>
+      <c r="C1542">
+        <v>4</v>
+      </c>
+      <c r="D1542">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1543">
+        <v>6</v>
+      </c>
+      <c r="B1543">
+        <v>2</v>
+      </c>
+      <c r="C1543">
+        <v>7</v>
+      </c>
+      <c r="D1543">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1544">
+        <v>4</v>
+      </c>
+      <c r="B1544">
+        <v>2</v>
+      </c>
+      <c r="C1544">
+        <v>3</v>
+      </c>
+      <c r="D1544">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1545">
+        <v>6</v>
+      </c>
+      <c r="B1545">
+        <v>2</v>
+      </c>
+      <c r="C1545">
+        <v>5</v>
+      </c>
+      <c r="D1545">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1546">
+        <v>5</v>
+      </c>
+      <c r="B1546">
+        <v>0</v>
+      </c>
+      <c r="C1546">
+        <v>5</v>
+      </c>
+      <c r="D1546">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1547">
+        <v>2</v>
+      </c>
+      <c r="B1547">
+        <v>1</v>
+      </c>
+      <c r="C1547">
+        <v>2</v>
+      </c>
+      <c r="D1547">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sum 23 week 10 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE46818D-C58A-48C2-BADA-2BDCE22E9829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA77EBE-2179-45E1-9174-39D37E2D3CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2078"/>
+  <dimension ref="A1:D2096"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2062" workbookViewId="0">
-      <selection activeCell="A2079" sqref="A2079"/>
+    <sheetView tabSelected="1" topLeftCell="A2080" workbookViewId="0">
+      <selection activeCell="A2097" sqref="A2097"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29467,6 +29467,258 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2079" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2079">
+        <v>3</v>
+      </c>
+      <c r="B2079">
+        <v>2</v>
+      </c>
+      <c r="C2079">
+        <v>3</v>
+      </c>
+      <c r="D2079">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2080" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2080">
+        <v>5</v>
+      </c>
+      <c r="B2080">
+        <v>2</v>
+      </c>
+      <c r="C2080">
+        <v>5</v>
+      </c>
+      <c r="D2080">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2081" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2081">
+        <v>3</v>
+      </c>
+      <c r="B2081">
+        <v>0</v>
+      </c>
+      <c r="C2081">
+        <v>3</v>
+      </c>
+      <c r="D2081">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2082" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2082">
+        <v>6</v>
+      </c>
+      <c r="B2082">
+        <v>2</v>
+      </c>
+      <c r="C2082">
+        <v>5</v>
+      </c>
+      <c r="D2082">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2083">
+        <v>5</v>
+      </c>
+      <c r="B2083">
+        <v>2</v>
+      </c>
+      <c r="C2083">
+        <v>5</v>
+      </c>
+      <c r="D2083">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2084">
+        <v>4</v>
+      </c>
+      <c r="B2084">
+        <v>3</v>
+      </c>
+      <c r="C2084">
+        <v>3</v>
+      </c>
+      <c r="D2084">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2085">
+        <v>4</v>
+      </c>
+      <c r="B2085">
+        <v>2</v>
+      </c>
+      <c r="C2085">
+        <v>5</v>
+      </c>
+      <c r="D2085">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2086">
+        <v>4</v>
+      </c>
+      <c r="B2086">
+        <v>2</v>
+      </c>
+      <c r="C2086">
+        <v>4</v>
+      </c>
+      <c r="D2086">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2087">
+        <v>6</v>
+      </c>
+      <c r="B2087">
+        <v>2</v>
+      </c>
+      <c r="C2087">
+        <v>5</v>
+      </c>
+      <c r="D2087">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2088">
+        <v>5</v>
+      </c>
+      <c r="B2088">
+        <v>3</v>
+      </c>
+      <c r="C2088">
+        <v>2</v>
+      </c>
+      <c r="D2088">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2089">
+        <v>5</v>
+      </c>
+      <c r="B2089">
+        <v>2</v>
+      </c>
+      <c r="C2089">
+        <v>5</v>
+      </c>
+      <c r="D2089">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2090">
+        <v>4</v>
+      </c>
+      <c r="B2090">
+        <v>3</v>
+      </c>
+      <c r="C2090">
+        <v>4</v>
+      </c>
+      <c r="D2090">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2091">
+        <v>2</v>
+      </c>
+      <c r="B2091">
+        <v>2</v>
+      </c>
+      <c r="C2091">
+        <v>5</v>
+      </c>
+      <c r="D2091">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2092">
+        <v>5</v>
+      </c>
+      <c r="B2092">
+        <v>2</v>
+      </c>
+      <c r="C2092">
+        <v>4</v>
+      </c>
+      <c r="D2092">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2093">
+        <v>4</v>
+      </c>
+      <c r="B2093">
+        <v>2</v>
+      </c>
+      <c r="C2093">
+        <v>3</v>
+      </c>
+      <c r="D2093">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2094">
+        <v>6</v>
+      </c>
+      <c r="B2094">
+        <v>2</v>
+      </c>
+      <c r="C2094">
+        <v>6</v>
+      </c>
+      <c r="D2094">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2095">
+        <v>4</v>
+      </c>
+      <c r="B2095">
+        <v>2</v>
+      </c>
+      <c r="C2095">
+        <v>4</v>
+      </c>
+      <c r="D2095">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2096">
+        <v>6</v>
+      </c>
+      <c r="B2096">
+        <v>2</v>
+      </c>
+      <c r="C2096">
+        <v>7</v>
+      </c>
+      <c r="D2096">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
week 6 inputs and github actions
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A295F961-F1B3-4D48-853D-1CB5B2675871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B455F2-CE1A-460F-B061-0D2DAB677F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="465" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2651"/>
+  <dimension ref="A1:D2671"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2641" workbookViewId="0">
-      <selection activeCell="F2663" sqref="F2663"/>
+    <sheetView tabSelected="1" topLeftCell="A2659" workbookViewId="0">
+      <selection activeCell="A2672" sqref="A2672"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37489,6 +37489,286 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2652" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2652">
+        <v>3</v>
+      </c>
+      <c r="B2652">
+        <v>3</v>
+      </c>
+      <c r="C2652">
+        <v>3</v>
+      </c>
+      <c r="D2652">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2653">
+        <v>5</v>
+      </c>
+      <c r="B2653">
+        <v>3</v>
+      </c>
+      <c r="C2653">
+        <v>4</v>
+      </c>
+      <c r="D2653">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2654">
+        <v>5</v>
+      </c>
+      <c r="B2654">
+        <v>2</v>
+      </c>
+      <c r="C2654">
+        <v>5</v>
+      </c>
+      <c r="D2654">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2655">
+        <v>4</v>
+      </c>
+      <c r="B2655">
+        <v>0</v>
+      </c>
+      <c r="C2655">
+        <v>6</v>
+      </c>
+      <c r="D2655">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2656">
+        <v>3</v>
+      </c>
+      <c r="B2656">
+        <v>0</v>
+      </c>
+      <c r="C2656">
+        <v>3</v>
+      </c>
+      <c r="D2656">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2657">
+        <v>6</v>
+      </c>
+      <c r="B2657">
+        <v>0</v>
+      </c>
+      <c r="C2657">
+        <v>7</v>
+      </c>
+      <c r="D2657">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2658">
+        <v>4</v>
+      </c>
+      <c r="B2658">
+        <v>2</v>
+      </c>
+      <c r="C2658">
+        <v>2</v>
+      </c>
+      <c r="D2658">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2659">
+        <v>4</v>
+      </c>
+      <c r="B2659">
+        <v>0</v>
+      </c>
+      <c r="C2659">
+        <v>5</v>
+      </c>
+      <c r="D2659">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2660">
+        <v>5</v>
+      </c>
+      <c r="B2660">
+        <v>2</v>
+      </c>
+      <c r="C2660">
+        <v>6</v>
+      </c>
+      <c r="D2660">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2661">
+        <v>4</v>
+      </c>
+      <c r="B2661">
+        <v>0</v>
+      </c>
+      <c r="C2661">
+        <v>3</v>
+      </c>
+      <c r="D2661">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2662">
+        <v>2</v>
+      </c>
+      <c r="B2662">
+        <v>0</v>
+      </c>
+      <c r="C2662">
+        <v>3</v>
+      </c>
+      <c r="D2662">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2663">
+        <v>4</v>
+      </c>
+      <c r="B2663">
+        <v>2</v>
+      </c>
+      <c r="C2663">
+        <v>5</v>
+      </c>
+      <c r="D2663">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2664">
+        <v>4</v>
+      </c>
+      <c r="B2664">
+        <v>2</v>
+      </c>
+      <c r="C2664">
+        <v>4</v>
+      </c>
+      <c r="D2664">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2665">
+        <v>5</v>
+      </c>
+      <c r="B2665">
+        <v>0</v>
+      </c>
+      <c r="C2665">
+        <v>3</v>
+      </c>
+      <c r="D2665">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2666">
+        <v>6</v>
+      </c>
+      <c r="B2666">
+        <v>0</v>
+      </c>
+      <c r="C2666">
+        <v>6</v>
+      </c>
+      <c r="D2666">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2667">
+        <v>3</v>
+      </c>
+      <c r="B2667">
+        <v>0</v>
+      </c>
+      <c r="C2667">
+        <v>3</v>
+      </c>
+      <c r="D2667">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2668">
+        <v>4</v>
+      </c>
+      <c r="B2668">
+        <v>0</v>
+      </c>
+      <c r="C2668">
+        <v>5</v>
+      </c>
+      <c r="D2668">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2669">
+        <v>3</v>
+      </c>
+      <c r="B2669">
+        <v>2</v>
+      </c>
+      <c r="C2669">
+        <v>4</v>
+      </c>
+      <c r="D2669">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2670">
+        <v>7</v>
+      </c>
+      <c r="B2670">
+        <v>3</v>
+      </c>
+      <c r="C2670">
+        <v>4</v>
+      </c>
+      <c r="D2670">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2671">
+        <v>3</v>
+      </c>
+      <c r="B2671">
+        <v>0</v>
+      </c>
+      <c r="C2671">
+        <v>7</v>
+      </c>
+      <c r="D2671">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
spring 24 week 8 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B455F2-CE1A-460F-B061-0D2DAB677F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55B1BE6-AA4D-4599-8933-C254C35E319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="465" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="465" windowWidth="16410" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2671"/>
+  <dimension ref="A1:D2704"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2659" workbookViewId="0">
-      <selection activeCell="A2672" sqref="A2672"/>
+    <sheetView tabSelected="1" topLeftCell="A2689" workbookViewId="0">
+      <selection activeCell="A2705" sqref="A2705"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37769,6 +37769,468 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2672" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2672">
+        <v>5</v>
+      </c>
+      <c r="B2672">
+        <v>0</v>
+      </c>
+      <c r="C2672">
+        <v>5</v>
+      </c>
+      <c r="D2672">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2673">
+        <v>4</v>
+      </c>
+      <c r="B2673">
+        <v>3</v>
+      </c>
+      <c r="C2673">
+        <v>3</v>
+      </c>
+      <c r="D2673">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2674">
+        <v>4</v>
+      </c>
+      <c r="B2674">
+        <v>0</v>
+      </c>
+      <c r="C2674">
+        <v>5</v>
+      </c>
+      <c r="D2674">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2675">
+        <v>3</v>
+      </c>
+      <c r="B2675">
+        <v>0</v>
+      </c>
+      <c r="C2675">
+        <v>3</v>
+      </c>
+      <c r="D2675">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2676">
+        <v>6</v>
+      </c>
+      <c r="B2676">
+        <v>0</v>
+      </c>
+      <c r="C2676">
+        <v>7</v>
+      </c>
+      <c r="D2676">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2677">
+        <v>2</v>
+      </c>
+      <c r="B2677">
+        <v>0</v>
+      </c>
+      <c r="C2677">
+        <v>3</v>
+      </c>
+      <c r="D2677">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2678">
+        <v>6</v>
+      </c>
+      <c r="B2678">
+        <v>2</v>
+      </c>
+      <c r="C2678">
+        <v>5</v>
+      </c>
+      <c r="D2678">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2679">
+        <v>5</v>
+      </c>
+      <c r="B2679">
+        <v>0</v>
+      </c>
+      <c r="C2679">
+        <v>7</v>
+      </c>
+      <c r="D2679">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2680">
+        <v>3</v>
+      </c>
+      <c r="B2680">
+        <v>2</v>
+      </c>
+      <c r="C2680">
+        <v>4</v>
+      </c>
+      <c r="D2680">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2681">
+        <v>6</v>
+      </c>
+      <c r="B2681">
+        <v>2</v>
+      </c>
+      <c r="C2681">
+        <v>4</v>
+      </c>
+      <c r="D2681">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2682">
+        <v>4</v>
+      </c>
+      <c r="B2682">
+        <v>0</v>
+      </c>
+      <c r="C2682">
+        <v>4</v>
+      </c>
+      <c r="D2682">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2683">
+        <v>6</v>
+      </c>
+      <c r="B2683">
+        <v>2</v>
+      </c>
+      <c r="C2683">
+        <v>3</v>
+      </c>
+      <c r="D2683">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2684">
+        <v>3</v>
+      </c>
+      <c r="B2684">
+        <v>0</v>
+      </c>
+      <c r="C2684">
+        <v>5</v>
+      </c>
+      <c r="D2684">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2685">
+        <v>4</v>
+      </c>
+      <c r="B2685">
+        <v>2</v>
+      </c>
+      <c r="C2685">
+        <v>4</v>
+      </c>
+      <c r="D2685">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2686">
+        <v>5</v>
+      </c>
+      <c r="B2686">
+        <v>2</v>
+      </c>
+      <c r="C2686">
+        <v>7</v>
+      </c>
+      <c r="D2686">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2687">
+        <v>4</v>
+      </c>
+      <c r="B2687">
+        <v>0</v>
+      </c>
+      <c r="C2687">
+        <v>4</v>
+      </c>
+      <c r="D2687">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2688">
+        <v>6</v>
+      </c>
+      <c r="B2688">
+        <v>2</v>
+      </c>
+      <c r="C2688">
+        <v>6</v>
+      </c>
+      <c r="D2688">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2689">
+        <v>5</v>
+      </c>
+      <c r="B2689">
+        <v>2</v>
+      </c>
+      <c r="C2689">
+        <v>4</v>
+      </c>
+      <c r="D2689">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2690">
+        <v>4</v>
+      </c>
+      <c r="B2690">
+        <v>0</v>
+      </c>
+      <c r="C2690">
+        <v>3</v>
+      </c>
+      <c r="D2690">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2691">
+        <v>4</v>
+      </c>
+      <c r="B2691">
+        <v>2</v>
+      </c>
+      <c r="C2691">
+        <v>7</v>
+      </c>
+      <c r="D2691">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2692">
+        <v>3</v>
+      </c>
+      <c r="B2692">
+        <v>3</v>
+      </c>
+      <c r="C2692">
+        <v>3</v>
+      </c>
+      <c r="D2692">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2693">
+        <v>4</v>
+      </c>
+      <c r="B2693">
+        <v>0</v>
+      </c>
+      <c r="C2693">
+        <v>5</v>
+      </c>
+      <c r="D2693">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2694">
+        <v>3</v>
+      </c>
+      <c r="B2694">
+        <v>1</v>
+      </c>
+      <c r="C2694">
+        <v>3</v>
+      </c>
+      <c r="D2694">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2695">
+        <v>4</v>
+      </c>
+      <c r="B2695">
+        <v>1</v>
+      </c>
+      <c r="C2695">
+        <v>4</v>
+      </c>
+      <c r="D2695">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2696">
+        <v>3</v>
+      </c>
+      <c r="B2696">
+        <v>0</v>
+      </c>
+      <c r="C2696">
+        <v>2</v>
+      </c>
+      <c r="D2696">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2697">
+        <v>3</v>
+      </c>
+      <c r="B2697">
+        <v>0</v>
+      </c>
+      <c r="C2697">
+        <v>4</v>
+      </c>
+      <c r="D2697">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2698">
+        <v>7</v>
+      </c>
+      <c r="B2698">
+        <v>2</v>
+      </c>
+      <c r="C2698">
+        <v>4</v>
+      </c>
+      <c r="D2698">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2699">
+        <v>6</v>
+      </c>
+      <c r="B2699">
+        <v>1</v>
+      </c>
+      <c r="C2699">
+        <v>6</v>
+      </c>
+      <c r="D2699">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2700">
+        <v>4</v>
+      </c>
+      <c r="B2700">
+        <v>1</v>
+      </c>
+      <c r="C2700">
+        <v>5</v>
+      </c>
+      <c r="D2700">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2701">
+        <v>4</v>
+      </c>
+      <c r="B2701">
+        <v>3</v>
+      </c>
+      <c r="C2701">
+        <v>4</v>
+      </c>
+      <c r="D2701">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2702">
+        <v>3</v>
+      </c>
+      <c r="B2702">
+        <v>0</v>
+      </c>
+      <c r="C2702">
+        <v>4</v>
+      </c>
+      <c r="D2702">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2703">
+        <v>6</v>
+      </c>
+      <c r="B2703">
+        <v>2</v>
+      </c>
+      <c r="C2703">
+        <v>5</v>
+      </c>
+      <c r="D2703">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2704">
+        <v>5</v>
+      </c>
+      <c r="B2704">
+        <v>1</v>
+      </c>
+      <c r="C2704">
+        <v>4</v>
+      </c>
+      <c r="D2704">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
spring 24 week 9 inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55B1BE6-AA4D-4599-8933-C254C35E319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62A31FA-DA7B-4B6C-8086-AF005BA5201D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="465" windowWidth="16410" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2704"/>
+  <dimension ref="A1:D2725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2689" workbookViewId="0">
-      <selection activeCell="A2705" sqref="A2705"/>
+    <sheetView tabSelected="1" topLeftCell="A2707" workbookViewId="0">
+      <selection activeCell="A2726" sqref="A2726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38231,6 +38231,300 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2705" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2705">
+        <v>6</v>
+      </c>
+      <c r="B2705">
+        <v>0</v>
+      </c>
+      <c r="C2705">
+        <v>5</v>
+      </c>
+      <c r="D2705">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2706">
+        <v>4</v>
+      </c>
+      <c r="B2706">
+        <v>3</v>
+      </c>
+      <c r="C2706">
+        <v>3</v>
+      </c>
+      <c r="D2706">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2707">
+        <v>3</v>
+      </c>
+      <c r="B2707">
+        <v>2</v>
+      </c>
+      <c r="C2707">
+        <v>2</v>
+      </c>
+      <c r="D2707">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2708">
+        <v>5</v>
+      </c>
+      <c r="B2708">
+        <v>1</v>
+      </c>
+      <c r="C2708">
+        <v>5</v>
+      </c>
+      <c r="D2708">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2709">
+        <v>5</v>
+      </c>
+      <c r="B2709">
+        <v>2</v>
+      </c>
+      <c r="C2709">
+        <v>6</v>
+      </c>
+      <c r="D2709">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2710">
+        <v>4</v>
+      </c>
+      <c r="B2710">
+        <v>0</v>
+      </c>
+      <c r="C2710">
+        <v>3</v>
+      </c>
+      <c r="D2710">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2711">
+        <v>4</v>
+      </c>
+      <c r="B2711">
+        <v>0</v>
+      </c>
+      <c r="C2711">
+        <v>4</v>
+      </c>
+      <c r="D2711">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2712">
+        <v>3</v>
+      </c>
+      <c r="B2712">
+        <v>1</v>
+      </c>
+      <c r="C2712">
+        <v>4</v>
+      </c>
+      <c r="D2712">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2713">
+        <v>6</v>
+      </c>
+      <c r="B2713">
+        <v>0</v>
+      </c>
+      <c r="C2713">
+        <v>5</v>
+      </c>
+      <c r="D2713">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2714">
+        <v>3</v>
+      </c>
+      <c r="B2714">
+        <v>0</v>
+      </c>
+      <c r="C2714">
+        <v>6</v>
+      </c>
+      <c r="D2714">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2715">
+        <v>7</v>
+      </c>
+      <c r="B2715">
+        <v>2</v>
+      </c>
+      <c r="C2715">
+        <v>3</v>
+      </c>
+      <c r="D2715">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2716">
+        <v>2</v>
+      </c>
+      <c r="B2716">
+        <v>0</v>
+      </c>
+      <c r="C2716">
+        <v>3</v>
+      </c>
+      <c r="D2716">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2717">
+        <v>4</v>
+      </c>
+      <c r="B2717">
+        <v>2</v>
+      </c>
+      <c r="C2717">
+        <v>5</v>
+      </c>
+      <c r="D2717">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2718">
+        <v>4</v>
+      </c>
+      <c r="B2718">
+        <v>2</v>
+      </c>
+      <c r="C2718">
+        <v>3</v>
+      </c>
+      <c r="D2718">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2719">
+        <v>5</v>
+      </c>
+      <c r="B2719">
+        <v>0</v>
+      </c>
+      <c r="C2719">
+        <v>5</v>
+      </c>
+      <c r="D2719">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2720">
+        <v>6</v>
+      </c>
+      <c r="B2720">
+        <v>0</v>
+      </c>
+      <c r="C2720">
+        <v>4</v>
+      </c>
+      <c r="D2720">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2721">
+        <v>4</v>
+      </c>
+      <c r="B2721">
+        <v>0</v>
+      </c>
+      <c r="C2721">
+        <v>4</v>
+      </c>
+      <c r="D2721">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2722">
+        <v>4</v>
+      </c>
+      <c r="B2722">
+        <v>0</v>
+      </c>
+      <c r="C2722">
+        <v>4</v>
+      </c>
+      <c r="D2722">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2723">
+        <v>5</v>
+      </c>
+      <c r="B2723">
+        <v>1</v>
+      </c>
+      <c r="C2723">
+        <v>6</v>
+      </c>
+      <c r="D2723">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2724">
+        <v>4</v>
+      </c>
+      <c r="B2724">
+        <v>2</v>
+      </c>
+      <c r="C2724">
+        <v>4</v>
+      </c>
+      <c r="D2724">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2725">
+        <v>6</v>
+      </c>
+      <c r="B2725">
+        <v>0</v>
+      </c>
+      <c r="C2725">
+        <v>4</v>
+      </c>
+      <c r="D2725">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
summer 24 week 3 8 ball inputs
</commit_message>
<xml_diff>
--- a/data/SLMatchups.xlsx
+++ b/data/SLMatchups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53cb9c05b082722/Documents/magic-8ball/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="13_ncr:1_{EF58B412-D997-42A7-9453-BBA9E1F751AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEDD67B4-3EF0-48B5-A2B2-89B6A9E9A31D}"/>
+  <xr:revisionPtr revIDLastSave="444" documentId="13_ncr:1_{EF58B412-D997-42A7-9453-BBA9E1F751AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB32C17-37D6-40F6-92CE-FE685D03EFF3}"/>
   <bookViews>
-    <workbookView xWindow="19875" yWindow="300" windowWidth="16410" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2875"/>
+  <dimension ref="A1:D2895"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2860" workbookViewId="0">
-      <selection activeCell="A2876" sqref="A2876"/>
+    <sheetView tabSelected="1" topLeftCell="A2887" workbookViewId="0">
+      <selection activeCell="A2896" sqref="A2896"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40629,6 +40629,286 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2876" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2876">
+        <v>4</v>
+      </c>
+      <c r="B2876">
+        <v>2</v>
+      </c>
+      <c r="C2876">
+        <v>4</v>
+      </c>
+      <c r="D2876">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2877">
+        <v>4</v>
+      </c>
+      <c r="B2877">
+        <v>2</v>
+      </c>
+      <c r="C2877">
+        <v>3</v>
+      </c>
+      <c r="D2877">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2878">
+        <v>4</v>
+      </c>
+      <c r="B2878">
+        <v>0</v>
+      </c>
+      <c r="C2878">
+        <v>3</v>
+      </c>
+      <c r="D2878">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2879" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2879">
+        <v>3</v>
+      </c>
+      <c r="B2879">
+        <v>2</v>
+      </c>
+      <c r="C2879">
+        <v>5</v>
+      </c>
+      <c r="D2879">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2880" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2880">
+        <v>5</v>
+      </c>
+      <c r="B2880">
+        <v>1</v>
+      </c>
+      <c r="C2880">
+        <v>7</v>
+      </c>
+      <c r="D2880">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2881" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2881">
+        <v>3</v>
+      </c>
+      <c r="B2881">
+        <v>1</v>
+      </c>
+      <c r="C2881">
+        <v>4</v>
+      </c>
+      <c r="D2881">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2882" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2882">
+        <v>2</v>
+      </c>
+      <c r="B2882">
+        <v>3</v>
+      </c>
+      <c r="C2882">
+        <v>2</v>
+      </c>
+      <c r="D2882">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2883" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2883">
+        <v>6</v>
+      </c>
+      <c r="B2883">
+        <v>2</v>
+      </c>
+      <c r="C2883">
+        <v>6</v>
+      </c>
+      <c r="D2883">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2884" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2884">
+        <v>6</v>
+      </c>
+      <c r="B2884">
+        <v>0</v>
+      </c>
+      <c r="C2884">
+        <v>6</v>
+      </c>
+      <c r="D2884">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2885" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2885">
+        <v>5</v>
+      </c>
+      <c r="B2885">
+        <v>1</v>
+      </c>
+      <c r="C2885">
+        <v>3</v>
+      </c>
+      <c r="D2885">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2886" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2886">
+        <v>4</v>
+      </c>
+      <c r="B2886">
+        <v>3</v>
+      </c>
+      <c r="C2886">
+        <v>5</v>
+      </c>
+      <c r="D2886">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2887" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2887">
+        <v>3</v>
+      </c>
+      <c r="B2887">
+        <v>2</v>
+      </c>
+      <c r="C2887">
+        <v>3</v>
+      </c>
+      <c r="D2887">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2888" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2888">
+        <v>5</v>
+      </c>
+      <c r="B2888">
+        <v>0</v>
+      </c>
+      <c r="C2888">
+        <v>3</v>
+      </c>
+      <c r="D2888">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2889" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2889">
+        <v>4</v>
+      </c>
+      <c r="B2889">
+        <v>3</v>
+      </c>
+      <c r="C2889">
+        <v>4</v>
+      </c>
+      <c r="D2889">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2890" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2890">
+        <v>5</v>
+      </c>
+      <c r="B2890">
+        <v>1</v>
+      </c>
+      <c r="C2890">
+        <v>5</v>
+      </c>
+      <c r="D2890">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2891" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2891">
+        <v>4</v>
+      </c>
+      <c r="B2891">
+        <v>0</v>
+      </c>
+      <c r="C2891">
+        <v>4</v>
+      </c>
+      <c r="D2891">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2892" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2892">
+        <v>4</v>
+      </c>
+      <c r="B2892">
+        <v>0</v>
+      </c>
+      <c r="C2892">
+        <v>5</v>
+      </c>
+      <c r="D2892">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2893" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2893">
+        <v>5</v>
+      </c>
+      <c r="B2893">
+        <v>0</v>
+      </c>
+      <c r="C2893">
+        <v>5</v>
+      </c>
+      <c r="D2893">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2894" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2894">
+        <v>4</v>
+      </c>
+      <c r="B2894">
+        <v>1</v>
+      </c>
+      <c r="C2894">
+        <v>6</v>
+      </c>
+      <c r="D2894">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2895" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2895">
+        <v>3</v>
+      </c>
+      <c r="B2895">
+        <v>1</v>
+      </c>
+      <c r="C2895">
+        <v>3</v>
+      </c>
+      <c r="D2895">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>